<commit_message>
added both curves on same plot
</commit_message>
<xml_diff>
--- a/results/correlation.xlsx
+++ b/results/correlation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\covid-19-india\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\covid-19-india\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61ADFF9-B9ED-44C1-99A3-42BA4C16872D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F7D42E-4BAD-437C-897D-691EE58522A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="2130" windowWidth="22050" windowHeight="15320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38437,8 +38437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="C236" sqref="C236"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>